<commit_message>
ADD - Event / United Front (EX)
</commit_message>
<xml_diff>
--- a/Event.xlsx
+++ b/Event.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aff98139d4bac41f/文件/DL/dragalia-data-track/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{60C86C0A-7BB3-4C91-9703-0BE219B0A686}"/>
+  <xr:revisionPtr revIDLastSave="212" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9FD9E7E9-3E43-409A-AC16-71F04EEA5391}"/>
   <bookViews>
-    <workbookView xWindow="29295" yWindow="2385" windowWidth="21600" windowHeight="13860" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
+    <workbookView xWindow="8865" yWindow="750" windowWidth="21600" windowHeight="13860" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
   </bookViews>
   <sheets>
     <sheet name="United Front" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>初級</t>
   </si>
@@ -65,10 +65,6 @@
     <t>上級</t>
   </si>
   <si>
-    <t>卡住的話就回去刷上一級的總力戰
-如果初級卡住，刷局地或前哨到2000 P開總力戰</t>
-  </si>
-  <si>
     <t>超級</t>
   </si>
   <si>
@@ -139,10 +135,6 @@
   </si>
   <si>
     <t>350000 P</t>
-  </si>
-  <si>
-    <t>故事進度(拿書)不影響任務進度(拿地圖)
-超級總力戰開啟後刷超級，上級雖然效率高，但是不會掉司令書</t>
   </si>
   <si>
     <t>超級掉落
@@ -165,6 +157,127 @@
   </si>
   <si>
     <t>已記錄場次</t>
+  </si>
+  <si>
+    <t>製作者:</t>
+  </si>
+  <si>
+    <t>協力者:</t>
+  </si>
+  <si>
+    <t>醜兔 / RaenonX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">歡迎轉載。轉載時，請勿修改本圖片的任何部分。 </t>
+  </si>
+  <si>
+    <t>Excel 可於 github.com/RaenonX/dragalia-data-track 下載</t>
+  </si>
+  <si>
+    <t>DamDaMean、Huang、Kevin Tu (大熊)、Saisa、河馬</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>卡住的話就回去刷上一級的總力戰</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+如果初級卡住，刷局地或前哨到2000 P開總力戰</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>超級總力戰開啟後刷超級，上級雖然效率高，但是不會掉司令書</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+故事進度(拿書)不影響任務進度(拿地圖)</t>
+    </r>
+  </si>
+  <si>
+    <t>EX要點</t>
+  </si>
+  <si>
+    <t>1人以下死亡</t>
+  </si>
+  <si>
+    <t>隊伍含火屬龍</t>
+  </si>
+  <si>
+    <t>隊伍含暗屬龍</t>
+  </si>
+  <si>
+    <t>隊伍不含風屬龍</t>
+  </si>
+  <si>
+    <t>隊伍不含光屬龍</t>
+  </si>
+  <si>
+    <t>120秒內通關</t>
+  </si>
+  <si>
+    <t>80秒內通關</t>
+  </si>
+  <si>
+    <t>60秒內通關</t>
+  </si>
+  <si>
+    <t>受傷1次以下</t>
+  </si>
+  <si>
+    <t>受傷2次以下</t>
+  </si>
+  <si>
+    <t>受傷3次以下</t>
+  </si>
+  <si>
+    <t>配組思路</t>
+  </si>
+  <si>
+    <t>搭配新增的四星護符(開場上盾)</t>
+  </si>
+  <si>
+    <t>編成順序：暗暗火火</t>
+  </si>
+  <si>
+    <t>若自動，挑選普攻範圍大的龍</t>
+  </si>
+  <si>
+    <t>若手動，挑選大招範圍大的龍</t>
+  </si>
+  <si>
+    <t>角色: 狗刀、法克、天才、二姊</t>
+  </si>
+  <si>
+    <t>推薦自動組合</t>
   </si>
   <si>
     <r>
@@ -178,33 +291,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>06/12 3:01 AM CDT</t>
+      <t>06/12 4:26 AM CDT</t>
     </r>
   </si>
   <si>
-    <t>製作者:</t>
-  </si>
-  <si>
-    <t>協力者:</t>
-  </si>
-  <si>
-    <t>醜兔 / RaenonX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">歡迎轉載。轉載時，請勿修改本圖片的任何部分。 </t>
-  </si>
-  <si>
-    <t>Excel 可於 github.com/RaenonX/dragalia-data-track 下載</t>
-  </si>
-  <si>
-    <t>DamDaMean、Huang、Kevin Tu (大熊)、Saisa、河馬</t>
+    <t>龍: 奈亞拉拖提普x2、狗妹x2</t>
+  </si>
+  <si>
+    <t>護符: (開場盾、70% HP ATK+)x4</t>
+  </si>
+  <si>
+    <t>EX - 含易取得條件</t>
+  </si>
+  <si>
+    <t>EX加分條件 (灰字 = 相對不易取得條件)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +361,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -281,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -400,11 +514,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -430,9 +581,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -460,25 +608,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -508,53 +674,56 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -931,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D545DF4-55DC-4582-810A-BD07097A5744}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="H9" sqref="A1:M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,114 +1113,114 @@
     <col min="5" max="5" width="9.140625" style="2"/>
     <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
+      <c r="A1" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
     </row>
     <row r="2" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23" t="s">
+      <c r="A2" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="42"/>
+    </row>
+    <row r="3" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="25"/>
-    </row>
-    <row r="3" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="30" t="s">
+      <c r="G3" s="37"/>
+      <c r="H3" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="32"/>
-      <c r="H3" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="32"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="37"/>
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="15" t="s">
+      <c r="I4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="J4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="K4" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="17" t="s">
-        <v>33</v>
-      </c>
       <c r="O4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1067,14 +1236,14 @@
         <f t="shared" ref="E5:E16" si="0">D5/C5</f>
         <v>100</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="9">
         <v>250</v>
       </c>
-      <c r="G5" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>28</v>
+      <c r="G5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="I5" s="6">
         <v>3</v>
@@ -1089,7 +1258,7 @@
       <c r="L5" s="6">
         <v>9</v>
       </c>
-      <c r="M5" s="11">
+      <c r="M5" s="10">
         <f>SUM($L$5:L5)</f>
         <v>9</v>
       </c>
@@ -1101,7 +1270,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
+      <c r="A6" s="38"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1115,14 +1284,14 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <v>2000</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="10" t="s">
+      <c r="G6" s="10" t="s">
         <v>15</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="I6" s="6">
         <v>3</v>
@@ -1137,7 +1306,7 @@
       <c r="L6" s="6">
         <v>12</v>
       </c>
-      <c r="M6" s="11">
+      <c r="M6" s="10">
         <f>SUM($L$5:L6)</f>
         <v>21</v>
       </c>
@@ -1149,7 +1318,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="33"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
@@ -1163,14 +1332,14 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <v>5600</v>
       </c>
-      <c r="G7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="10" t="s">
         <v>16</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="I7" s="6">
         <v>5</v>
@@ -1185,7 +1354,7 @@
       <c r="L7" s="6">
         <v>25</v>
       </c>
-      <c r="M7" s="11">
+      <c r="M7" s="10">
         <f>SUM($L$5:L7)</f>
         <v>46</v>
       </c>
@@ -1197,7 +1366,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="39" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1213,14 +1382,14 @@
         <f t="shared" si="0"/>
         <v>116.66666666666667</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <v>8000</v>
       </c>
-      <c r="G8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>29</v>
+      <c r="G8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="I8" s="6">
         <v>1</v>
@@ -1235,7 +1404,7 @@
       <c r="L8" s="6">
         <v>6</v>
       </c>
-      <c r="M8" s="11">
+      <c r="M8" s="10">
         <f>SUM($L$5:L8)</f>
         <v>52</v>
       </c>
@@ -1247,7 +1416,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
@@ -1261,14 +1430,14 @@
         <f t="shared" si="0"/>
         <v>128.57142857142858</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="9">
         <v>25000</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>17</v>
+      <c r="G9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="I9" s="6">
         <v>1</v>
@@ -1283,7 +1452,7 @@
       <c r="L9" s="6">
         <v>7</v>
       </c>
-      <c r="M9" s="11">
+      <c r="M9" s="10">
         <f>SUM($L$5:L9)</f>
         <v>59</v>
       </c>
@@ -1295,7 +1464,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="34"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1309,14 +1478,14 @@
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="9">
         <v>58000</v>
       </c>
-      <c r="G10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>18</v>
+      <c r="G10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="I10" s="6">
         <v>24</v>
@@ -1332,7 +1501,7 @@
         <f>24*8</f>
         <v>192</v>
       </c>
-      <c r="M10" s="11">
+      <c r="M10" s="10">
         <f>SUM($L$5:L10)</f>
         <v>251</v>
       </c>
@@ -1344,7 +1513,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="38" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1360,14 +1529,14 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="9">
         <v>90000</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>30</v>
+      <c r="G11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="I11" s="6">
         <v>1</v>
@@ -1382,7 +1551,7 @@
       <c r="L11" s="6">
         <v>10</v>
       </c>
-      <c r="M11" s="11">
+      <c r="M11" s="10">
         <f>SUM($L$5:L11)</f>
         <v>261</v>
       </c>
@@ -1394,7 +1563,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="33"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1408,14 +1577,14 @@
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="11">
         <v>160000</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>19</v>
+      <c r="G12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="I12" s="6">
         <v>1</v>
@@ -1430,7 +1599,7 @@
       <c r="L12" s="6">
         <v>12</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="10">
         <f>SUM($L$5:L12)</f>
         <v>273</v>
       </c>
@@ -1442,7 +1611,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="33"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1457,13 +1626,13 @@
         <v>357.14285714285717</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="I13" s="6">
         <v>19</v>
@@ -1479,7 +1648,7 @@
         <f>14*19</f>
         <v>266</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="10">
         <f>SUM($L$5:L13)</f>
         <v>539</v>
       </c>
@@ -1491,8 +1660,8 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
-        <v>11</v>
+      <c r="A14" s="39" t="s">
+        <v>10</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>5</v>
@@ -1507,15 +1676,15 @@
         <f t="shared" si="0"/>
         <v>187.5</v>
       </c>
-      <c r="F14" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="29">
+      <c r="F14" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="34">
         <f>SUM(O:O)/SUM(P:P)</f>
-        <v>2.4117647058823528</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>31</v>
+        <v>2.3857142857142857</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="I14" s="6">
         <v>1</v>
@@ -1530,13 +1699,19 @@
       <c r="L14" s="6">
         <v>16</v>
       </c>
-      <c r="M14" s="11">
+      <c r="M14" s="10">
         <f>SUM($L$5:L14)</f>
         <v>555</v>
       </c>
+      <c r="O14" s="1">
+        <v>30</v>
+      </c>
+      <c r="P14" s="1">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
@@ -1550,10 +1725,10 @@
         <f t="shared" si="0"/>
         <v>222.22222222222223</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="10" t="s">
-        <v>21</v>
+      <c r="F15" s="33"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="I15" s="6">
         <v>1</v>
@@ -1568,13 +1743,19 @@
       <c r="L15" s="6">
         <v>18</v>
       </c>
-      <c r="M15" s="11">
+      <c r="M15" s="10">
         <f>SUM($L$5:L15)</f>
         <v>573</v>
       </c>
+      <c r="O15" s="1">
+        <v>99</v>
+      </c>
+      <c r="P15" s="1">
+        <v>42</v>
+      </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="34"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="8" t="s">
         <v>7</v>
       </c>
@@ -1588,172 +1769,308 @@
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="10" t="s">
-        <v>22</v>
+      <c r="F16" s="33"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="I16" s="6">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="J16" s="6">
         <f>I16*D16</f>
-        <v>1162000</v>
+        <v>1057000</v>
       </c>
       <c r="K16" s="6">
         <f>SUM($J$5:J16)</f>
-        <v>1323200</v>
+        <v>1218200</v>
       </c>
       <c r="L16" s="6">
         <f>I16*C16</f>
-        <v>3320</v>
-      </c>
-      <c r="M16" s="11">
+        <v>3020</v>
+      </c>
+      <c r="M16" s="10">
         <f>SUM($L$5:L16)</f>
-        <v>3893</v>
+        <v>3593</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="49"/>
+      <c r="C17" s="6">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6">
+        <v>12700</v>
+      </c>
+      <c r="E17" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="9">
+      <c r="G17" s="10">
+        <f>SUM(O:O)</f>
+        <v>334</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="6">
+        <f>_xlfn.FLOOR.MATH(I16/G14)</f>
+        <v>63</v>
+      </c>
+      <c r="J17" s="6">
+        <f>I17*D17</f>
+        <v>800100</v>
+      </c>
+      <c r="K17" s="6">
+        <f>SUM($J$5:J17)</f>
+        <v>2018300</v>
+      </c>
+      <c r="L17" s="6">
         <v>0</v>
       </c>
-      <c r="D17" s="9">
-        <v>10000</v>
-      </c>
-      <c r="E17" s="19" t="s">
+      <c r="M17" s="10">
+        <f>SUM($L$5:L17)</f>
+        <v>3593</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" s="53"/>
+      <c r="M18" s="54"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="43"/>
+      <c r="B19" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="47"/>
+      <c r="F19" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="55"/>
+      <c r="H19" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="50"/>
+      <c r="M19" s="51"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="43"/>
+      <c r="B20" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="47"/>
+      <c r="F20" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="55"/>
+      <c r="H20" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" s="47"/>
+      <c r="M20" s="51"/>
+    </row>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="43"/>
+      <c r="B21" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="55"/>
+      <c r="D21" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="47"/>
+      <c r="F21" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="55"/>
+      <c r="H21" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="L21" s="47"/>
+      <c r="M21" s="51"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="30"/>
+      <c r="B22" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="56"/>
+      <c r="D22" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="52"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="26"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="23"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="13">
-        <f>SUM(O:O)</f>
-        <v>205</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="9">
-        <f>_xlfn.FLOOR.MATH(I16/G14)</f>
-        <v>68</v>
-      </c>
-      <c r="J17" s="9">
-        <f>I17*D17</f>
-        <v>680000</v>
-      </c>
-      <c r="K17" s="9">
-        <f>SUM($J$5:J17)</f>
-        <v>2003200</v>
-      </c>
-      <c r="L17" s="9">
-        <v>0</v>
-      </c>
-      <c r="M17" s="13">
-        <f>SUM($L$5:L17)</f>
-        <v>3893</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="36" t="s">
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="26"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="29"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-      <c r="L18" s="37"/>
-      <c r="M18" s="38"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="47"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="40"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="41"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="48" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="50"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="43"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="44"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A22:G22"/>
-    <mergeCell ref="H22:M22"/>
-    <mergeCell ref="A18:M18"/>
-    <mergeCell ref="A19:M19"/>
-    <mergeCell ref="A20:M20"/>
-    <mergeCell ref="A21:M21"/>
+  <mergeCells count="43">
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B18:G18"/>
     <mergeCell ref="A17:B17"/>
-    <mergeCell ref="H2:M2"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="F14:F16"/>
     <mergeCell ref="G14:G16"/>
@@ -1764,9 +2081,16 @@
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A26:M26"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:E17 E23:E1048576">
+  <conditionalFormatting sqref="E28:E1048576 E4:E17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
FIX - Event / United Front layout
</commit_message>
<xml_diff>
--- a/Event.xlsx
+++ b/Event.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aff98139d4bac41f/文件/DL/dragalia-data-track/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="212" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9FD9E7E9-3E43-409A-AC16-71F04EEA5391}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C2049EE5-931C-45ED-97E3-CA222C21CF8B}"/>
   <bookViews>
-    <workbookView xWindow="8865" yWindow="750" windowWidth="21600" windowHeight="13860" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
+    <workbookView xWindow="4590" yWindow="870" windowWidth="21600" windowHeight="13860" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
   </bookViews>
   <sheets>
     <sheet name="United Front" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
   <si>
     <t>初級</t>
   </si>
@@ -262,24 +262,6 @@
     <t>配組思路</t>
   </si>
   <si>
-    <t>搭配新增的四星護符(開場上盾)</t>
-  </si>
-  <si>
-    <t>編成順序：暗暗火火</t>
-  </si>
-  <si>
-    <t>若自動，挑選普攻範圍大的龍</t>
-  </si>
-  <si>
-    <t>若手動，挑選大招範圍大的龍</t>
-  </si>
-  <si>
-    <t>角色: 狗刀、法克、天才、二姊</t>
-  </si>
-  <si>
-    <t>推薦自動組合</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">新迎擊戰 簡表 </t>
     </r>
@@ -295,9 +277,6 @@
     </r>
   </si>
   <si>
-    <t>龍: 奈亞拉拖提普x2、狗妹x2</t>
-  </si>
-  <si>
     <t>護符: (開場盾、70% HP ATK+)x4</t>
   </si>
   <si>
@@ -305,13 +284,101 @@
   </si>
   <si>
     <t>EX加分條件 (灰字 = 相對不易取得條件)</t>
+  </si>
+  <si>
+    <t>受傷次數條件高機率全部達成</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">角色: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>狗刀、法克</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>天才、二姊</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">龍: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>奈亞拉拖提普x2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>狗妹x2</t>
+    </r>
+  </si>
+  <si>
+    <t>推薦全自動組合</t>
+  </si>
+  <si>
+    <t>- 搭配新增的四星護符(開場上盾)</t>
+  </si>
+  <si>
+    <t>- 編成順序：暗暗火火</t>
+  </si>
+  <si>
+    <t>- 若自動，挑選普攻範圍大的龍</t>
+  </si>
+  <si>
+    <t>- 若手動，挑選大招範圍大的龍</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,6 +435,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -395,7 +483,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -551,11 +639,110 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -608,6 +795,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -616,6 +848,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -626,15 +867,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -644,86 +876,59 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1103,7 +1308,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="A1:M27"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,61 +1323,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
+      <c r="A1" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41" t="s">
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="42"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="32"/>
     </row>
     <row r="3" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="35" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="37"/>
-      <c r="H3" s="35" t="s">
+      <c r="G3" s="27"/>
+      <c r="H3" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="37"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="27"/>
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
@@ -1220,7 +1425,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="28" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1270,7 +1475,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="38"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1318,7 +1523,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
@@ -1366,7 +1571,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="29" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1416,7 +1621,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
@@ -1464,7 +1669,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="39"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1513,7 +1718,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="28" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1563,7 +1768,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1611,7 +1816,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1660,7 +1865,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="29" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1676,10 +1881,10 @@
         <f t="shared" si="0"/>
         <v>187.5</v>
       </c>
-      <c r="F14" s="32" t="s">
+      <c r="F14" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="24">
         <f>SUM(O:O)/SUM(P:P)</f>
         <v>2.3857142857142857</v>
       </c>
@@ -1711,7 +1916,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
@@ -1725,8 +1930,8 @@
         <f t="shared" si="0"/>
         <v>222.22222222222223</v>
       </c>
-      <c r="F15" s="33"/>
-      <c r="G15" s="34"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="24"/>
       <c r="H15" s="9" t="s">
         <v>20</v>
       </c>
@@ -1755,7 +1960,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="8" t="s">
         <v>7</v>
       </c>
@@ -1769,8 +1974,8 @@
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
-      <c r="F16" s="33"/>
-      <c r="G16" s="34"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="24"/>
       <c r="H16" s="9" t="s">
         <v>21</v>
       </c>
@@ -1795,20 +2000,20 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="49"/>
+      <c r="A17" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="21"/>
       <c r="C17" s="6">
         <v>0</v>
       </c>
       <c r="D17" s="6">
         <v>12700</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="E17" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="45" t="s">
+      <c r="F17" s="19" t="s">
         <v>40</v>
       </c>
       <c r="G17" s="10">
@@ -1839,237 +2044,221 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+      <c r="A18" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="53" t="s">
+      <c r="B18" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="45"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" s="45"/>
+      <c r="M18" s="47"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="61"/>
+      <c r="B19" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="37"/>
+      <c r="F19" s="57" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="58"/>
+      <c r="H19" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="37"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="L19" s="48"/>
+      <c r="M19" s="38"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="61"/>
+      <c r="B20" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="37"/>
+      <c r="F20" s="57" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="58"/>
+      <c r="H20" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" s="37"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="L20" s="37"/>
+      <c r="M20" s="38"/>
+    </row>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="61"/>
+      <c r="B21" s="57" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="57"/>
+      <c r="D21" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="37"/>
+      <c r="F21" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="58"/>
+      <c r="H21" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="L18" s="53"/>
-      <c r="M18" s="54"/>
-    </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="47"/>
-      <c r="F19" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" s="55"/>
-      <c r="H19" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="50" t="s">
+      <c r="I21" s="37"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="L21" s="37"/>
+      <c r="M21" s="38"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="62"/>
+      <c r="B22" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="59"/>
+      <c r="D22" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="I22" s="46"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="L19" s="50"/>
-      <c r="M19" s="51"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43"/>
-      <c r="B20" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="47"/>
-      <c r="F20" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="55"/>
-      <c r="H20" s="47" t="s">
-        <v>63</v>
-      </c>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="L20" s="47"/>
-      <c r="M20" s="51"/>
-    </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="55"/>
-      <c r="D21" s="47" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="47"/>
-      <c r="F21" s="55" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="55"/>
-      <c r="H21" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="L21" s="47"/>
-      <c r="M21" s="51"/>
-    </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="56" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="56"/>
-      <c r="D22" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="52"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="50"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="26"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="L23" s="37"/>
+      <c r="M23" s="38"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="23"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="41"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="26"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="37"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="38"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+      <c r="A26" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="29"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
+      <c r="M26" s="44"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19" t="s">
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="20"/>
+      <c r="I27" s="34"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="34"/>
+      <c r="L27" s="34"/>
+      <c r="M27" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A26:M26"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="F14:F16"/>
@@ -2083,12 +2272,30 @@
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="G2:M2"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="A23:M23"/>
-    <mergeCell ref="A24:M24"/>
-    <mergeCell ref="A25:M25"/>
-    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
   </mergeCells>
   <conditionalFormatting sqref="E28:E1048576 E4:E17">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
FIX - Event / United Front - Recommended FA
</commit_message>
<xml_diff>
--- a/Event.xlsx
+++ b/Event.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aff98139d4bac41f/文件/DL/dragalia-data-track/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="234" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C2049EE5-931C-45ED-97E3-CA222C21CF8B}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{02A8A812-E789-4C27-9840-C84F62640E69}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="870" windowWidth="21600" windowHeight="13860" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
+    <workbookView xWindow="4935" yWindow="1215" windowWidth="21600" windowHeight="13860" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
   </bookViews>
   <sheets>
     <sheet name="United Front" sheetId="1" r:id="rId1"/>
@@ -287,41 +287,6 @@
   </si>
   <si>
     <t>受傷次數條件高機率全部達成</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">角色: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>狗刀、法克</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>、</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>天才、二姊</t>
-    </r>
   </si>
   <si>
     <r>
@@ -372,6 +337,41 @@
   </si>
   <si>
     <t>- 若手動，挑選大招範圍大的龍</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">角色: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>狗刀、法克</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>兔短、二姊</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -801,6 +801,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -840,66 +876,51 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -908,27 +929,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1308,7 +1308,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,61 +1323,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="32"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="44"/>
     </row>
     <row r="3" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="25" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="25" t="s">
+      <c r="G3" s="39"/>
+      <c r="H3" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="27"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="39"/>
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
@@ -1425,7 +1425,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="40" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1475,7 +1475,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1523,7 +1523,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="40"/>
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
@@ -1571,7 +1571,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="41" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1621,7 +1621,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
@@ -1669,7 +1669,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1718,7 +1718,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="40" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1768,7 +1768,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
+      <c r="A12" s="40"/>
       <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1816,7 +1816,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
+      <c r="A13" s="40"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1865,7 +1865,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="41" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1881,10 +1881,10 @@
         <f t="shared" si="0"/>
         <v>187.5</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="36">
         <f>SUM(O:O)/SUM(P:P)</f>
         <v>2.3857142857142857</v>
       </c>
@@ -1916,7 +1916,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
@@ -1930,8 +1930,8 @@
         <f t="shared" si="0"/>
         <v>222.22222222222223</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="24"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="36"/>
       <c r="H15" s="9" t="s">
         <v>20</v>
       </c>
@@ -1960,7 +1960,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="8" t="s">
         <v>7</v>
       </c>
@@ -1974,8 +1974,8 @@
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="24"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="36"/>
       <c r="H16" s="9" t="s">
         <v>21</v>
       </c>
@@ -2000,10 +2000,10 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="6">
         <v>0</v>
       </c>
@@ -2044,221 +2044,239 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="51" t="s">
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="I18" s="45"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="45" t="s">
+      <c r="I18" s="53"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="L18" s="53"/>
+      <c r="M18" s="59"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="50"/>
+      <c r="B19" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E19" s="24"/>
+      <c r="F19" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="47"/>
+      <c r="H19" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="L18" s="45"/>
-      <c r="M18" s="47"/>
-    </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="61"/>
-      <c r="B19" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="37"/>
-      <c r="F19" s="57" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" s="58"/>
-      <c r="H19" s="53" t="s">
+      <c r="I19" s="24"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="L19" s="56"/>
+      <c r="M19" s="25"/>
+    </row>
+    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="50"/>
+      <c r="B20" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="47"/>
+      <c r="H20" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="48" t="s">
+      <c r="I20" s="24"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="L19" s="48"/>
-      <c r="M19" s="38"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="61"/>
-      <c r="B20" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="57" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="58"/>
-      <c r="H20" s="53" t="s">
+      <c r="L20" s="24"/>
+      <c r="M20" s="25"/>
+    </row>
+    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="50"/>
+      <c r="B21" s="46" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="46"/>
+      <c r="D21" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="47"/>
+      <c r="H21" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="L20" s="37"/>
-      <c r="M20" s="38"/>
-    </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="61"/>
-      <c r="B21" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="57"/>
-      <c r="D21" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="37"/>
-      <c r="F21" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="58"/>
-      <c r="H21" s="53" t="s">
+      <c r="I21" s="24"/>
+      <c r="J21" s="61"/>
+      <c r="K21" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="L21" s="24"/>
+      <c r="M21" s="25"/>
+    </row>
+    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="51"/>
+      <c r="B22" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="52"/>
+      <c r="D22" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="I21" s="37"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="L21" s="37"/>
-      <c r="M21" s="38"/>
-    </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="62"/>
-      <c r="B22" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="56"/>
-      <c r="H22" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="I22" s="46"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="49" t="s">
+      <c r="I22" s="45"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="57" t="s">
         <v>66</v>
       </c>
-      <c r="L22" s="49"/>
-      <c r="M22" s="50"/>
+      <c r="L22" s="57"/>
+      <c r="M22" s="58"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="38"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="25"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="41"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="28"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="37"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="38"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="25"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="44"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="30"/>
+      <c r="K26" s="30"/>
+      <c r="L26" s="30"/>
+      <c r="M26" s="31"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34" t="s">
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="35"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="A23:M23"/>
-    <mergeCell ref="A24:M24"/>
-    <mergeCell ref="A25:M25"/>
-    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="F14:F16"/>
@@ -2272,30 +2290,12 @@
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="G2:M2"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A26:M26"/>
   </mergeCells>
   <conditionalFormatting sqref="E28:E1048576 E4:E17">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
FIX - SS / BUF
</commit_message>
<xml_diff>
--- a/Event.xlsx
+++ b/Event.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aff98139d4bac41f/文件/DL/dragalia-data-track/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{02A8A812-E789-4C27-9840-C84F62640E69}"/>
+  <xr:revisionPtr revIDLastSave="262" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6702D43F-10D1-4792-8070-FFE81821B341}"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="1215" windowWidth="21600" windowHeight="13860" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
+    <workbookView xWindow="29010" yWindow="360" windowWidth="21600" windowHeight="13890" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
   </bookViews>
   <sheets>
     <sheet name="United Front" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
   <si>
     <t>初級</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>Excel 可於 github.com/RaenonX/dragalia-data-track 下載</t>
-  </si>
-  <si>
-    <t>DamDaMean、Huang、Kevin Tu (大熊)、Saisa、河馬</t>
   </si>
   <si>
     <r>
@@ -372,6 +369,12 @@
       </rPr>
       <t>兔短、二姊</t>
     </r>
+  </si>
+  <si>
+    <t>DamDaMean、Huang、Kevin Tu (大熊)、Moto、Saisa、河馬、椪柑</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -876,34 +879,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1308,7 +1311,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,7 +1327,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="34"/>
       <c r="C1" s="34"/>
@@ -1341,7 +1344,7 @@
     </row>
     <row r="2" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="43"/>
       <c r="C2" s="43"/>
@@ -1349,7 +1352,7 @@
       <c r="E2" s="43"/>
       <c r="F2" s="43"/>
       <c r="G2" s="43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H2" s="43"/>
       <c r="I2" s="43"/>
@@ -1886,7 +1889,7 @@
       </c>
       <c r="G14" s="36">
         <f>SUM(O:O)/SUM(P:P)</f>
-        <v>2.3857142857142857</v>
+        <v>2.2682926829268291</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>30</v>
@@ -1980,28 +1983,34 @@
         <v>21</v>
       </c>
       <c r="I16" s="6">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J16" s="6">
         <f>I16*D16</f>
-        <v>1057000</v>
+        <v>1043000</v>
       </c>
       <c r="K16" s="6">
         <f>SUM($J$5:J16)</f>
-        <v>1218200</v>
+        <v>1204200</v>
       </c>
       <c r="L16" s="6">
         <f>I16*C16</f>
-        <v>3020</v>
+        <v>2980</v>
       </c>
       <c r="M16" s="10">
         <f>SUM($L$5:L16)</f>
-        <v>3593</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>3553</v>
+      </c>
+      <c r="O16" s="1">
+        <v>30</v>
+      </c>
+      <c r="P16" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="6">
@@ -2018,153 +2027,189 @@
       </c>
       <c r="G17" s="10">
         <f>SUM(O:O)</f>
-        <v>334</v>
+        <v>651</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>38</v>
       </c>
       <c r="I17" s="6">
         <f>_xlfn.FLOOR.MATH(I16/G14)</f>
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J17" s="6">
         <f>I17*D17</f>
-        <v>800100</v>
+        <v>825500</v>
       </c>
       <c r="K17" s="6">
         <f>SUM($J$5:J17)</f>
-        <v>2018300</v>
+        <v>2029700</v>
       </c>
       <c r="L17" s="6">
         <v>0</v>
       </c>
       <c r="M17" s="10">
         <f>SUM($L$5:L17)</f>
-        <v>3593</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+        <v>3553</v>
+      </c>
+      <c r="O17" s="1">
+        <v>10</v>
+      </c>
+      <c r="P17" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="50"/>
+      <c r="J18" s="51"/>
+      <c r="K18" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="L18" s="50"/>
+      <c r="M18" s="59"/>
+      <c r="O18" s="1">
+        <v>20</v>
+      </c>
+      <c r="P18" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="46"/>
+      <c r="B19" s="24" t="s">
         <v>49</v>
-      </c>
-      <c r="B18" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="I18" s="53"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="L18" s="53"/>
-      <c r="M18" s="59"/>
-    </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="24" t="s">
-        <v>50</v>
       </c>
       <c r="C19" s="24"/>
       <c r="D19" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="24"/>
-      <c r="F19" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19" s="47"/>
+      <c r="F19" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="53"/>
       <c r="H19" s="60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I19" s="24"/>
       <c r="J19" s="61"/>
       <c r="K19" s="56" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L19" s="56"/>
       <c r="M19" s="25"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
+      <c r="O19" s="1">
+        <v>30</v>
+      </c>
+      <c r="P19" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="46"/>
       <c r="B20" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="24"/>
       <c r="D20" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="24"/>
-      <c r="F20" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20" s="47"/>
+      <c r="F20" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="53"/>
       <c r="H20" s="60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I20" s="24"/>
       <c r="J20" s="61"/>
       <c r="K20" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L20" s="24"/>
       <c r="M20" s="25"/>
-    </row>
-    <row r="21" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="46"/>
+      <c r="O20" s="1">
+        <v>99</v>
+      </c>
+      <c r="P20" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="46"/>
+      <c r="B21" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="48"/>
       <c r="D21" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="24"/>
-      <c r="F21" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="47"/>
+      <c r="F21" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="53"/>
       <c r="H21" s="60" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I21" s="24"/>
       <c r="J21" s="61"/>
       <c r="K21" s="24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L21" s="24"/>
       <c r="M21" s="25"/>
-    </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
-      <c r="B22" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="48"/>
+      <c r="O21" s="1">
+        <v>25</v>
+      </c>
+      <c r="P21" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="47"/>
+      <c r="B22" s="49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="49"/>
+      <c r="D22" s="52" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="54"/>
       <c r="H22" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="I22" s="45"/>
-      <c r="J22" s="48"/>
+        <v>71</v>
+      </c>
+      <c r="I22" s="52"/>
+      <c r="J22" s="54"/>
       <c r="K22" s="57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L22" s="57"/>
       <c r="M22" s="58"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O22" s="1">
+        <v>4</v>
+      </c>
+      <c r="P22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>42</v>
       </c>
@@ -2180,10 +2225,16 @@
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
       <c r="M23" s="25"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O23" s="1">
+        <v>99</v>
+      </c>
+      <c r="P23" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
@@ -2197,8 +2248,11 @@
       <c r="K24" s="27"/>
       <c r="L24" s="27"/>
       <c r="M24" s="28"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P24" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>41</v>
       </c>
@@ -2215,7 +2269,7 @@
       <c r="L25" s="24"/>
       <c r="M25" s="25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="29" t="s">
         <v>43</v>
       </c>
@@ -2232,7 +2286,7 @@
       <c r="L26" s="30"/>
       <c r="M26" s="31"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
IMP - Event / UnitedFront
</commit_message>
<xml_diff>
--- a/Event.xlsx
+++ b/Event.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aff98139d4bac41f/文件/DL/dragalia-data-track/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="262" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6702D43F-10D1-4792-8070-FFE81821B341}"/>
+  <xr:revisionPtr revIDLastSave="266" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3D80C619-B7BC-4D6D-9BCB-1C5C81ED0368}"/>
   <bookViews>
-    <workbookView xWindow="29010" yWindow="360" windowWidth="21600" windowHeight="13890" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
+    <workbookView xWindow="4950" yWindow="1080" windowWidth="20820" windowHeight="13890" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
   </bookViews>
   <sheets>
     <sheet name="United Front" sheetId="1" r:id="rId1"/>
@@ -257,24 +257,6 @@
   </si>
   <si>
     <t>配組思路</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">新迎擊戰 簡表 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>06/12 4:26 AM CDT</t>
-    </r>
-  </si>
-  <si>
-    <t>護符: (開場盾、70% HP ATK+)x4</t>
   </si>
   <si>
     <t>EX - 含易取得條件</t>
@@ -375,6 +357,24 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>護符: 盾、70% HP ATK+/古老盟約</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">新迎擊戰 簡表 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>06/13 5:23 AM CDT</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -804,6 +804,105 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -816,12 +915,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -839,99 +932,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1311,7 +1311,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="G2" sqref="A1:M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,61 +1326,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
+      <c r="A1" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="44"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="52"/>
     </row>
     <row r="3" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="37" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="39"/>
-      <c r="H3" s="37" t="s">
+      <c r="G3" s="47"/>
+      <c r="H3" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="39"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="47"/>
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
@@ -1428,7 +1428,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="48" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1478,7 +1478,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
+      <c r="A6" s="48"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1526,7 +1526,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +1574,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="49" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1624,7 +1624,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
@@ -1672,7 +1672,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1721,7 +1721,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="48" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1771,7 +1771,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1819,7 +1819,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1868,7 +1868,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="49" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1884,10 +1884,10 @@
         <f t="shared" si="0"/>
         <v>187.5</v>
       </c>
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="36">
+      <c r="G14" s="44">
         <f>SUM(O:O)/SUM(P:P)</f>
         <v>2.2682926829268291</v>
       </c>
@@ -1919,7 +1919,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
@@ -1933,8 +1933,8 @@
         <f t="shared" si="0"/>
         <v>222.22222222222223</v>
       </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="36"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="44"/>
       <c r="H15" s="9" t="s">
         <v>20</v>
       </c>
@@ -1963,7 +1963,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="8" t="s">
         <v>7</v>
       </c>
@@ -1977,8 +1977,8 @@
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="36"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="44"/>
       <c r="H16" s="9" t="s">
         <v>21</v>
       </c>
@@ -2009,10 +2009,10 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" s="33"/>
+      <c r="A17" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="41"/>
       <c r="C17" s="6">
         <v>0</v>
       </c>
@@ -2059,27 +2059,27 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="50"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="55" t="s">
+      <c r="B18" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I18" s="50"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="L18" s="50"/>
-      <c r="M18" s="59"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="L18" s="21"/>
+      <c r="M18" s="28"/>
       <c r="O18" s="1">
         <v>20</v>
       </c>
@@ -2088,29 +2088,29 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46"/>
-      <c r="B19" s="24" t="s">
+      <c r="A19" s="35"/>
+      <c r="B19" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24" t="s">
+      <c r="C19" s="25"/>
+      <c r="D19" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="24"/>
-      <c r="F19" s="48" t="s">
+      <c r="E19" s="25"/>
+      <c r="F19" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="53"/>
-      <c r="H19" s="60" t="s">
-        <v>68</v>
-      </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="56" t="s">
-        <v>72</v>
-      </c>
-      <c r="L19" s="56"/>
-      <c r="M19" s="25"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="25"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" s="23"/>
+      <c r="M19" s="24"/>
       <c r="O19" s="1">
         <v>30</v>
       </c>
@@ -2119,29 +2119,29 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="46"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="35"/>
+      <c r="B20" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24" t="s">
+      <c r="C20" s="25"/>
+      <c r="D20" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="48" t="s">
+      <c r="E20" s="25"/>
+      <c r="F20" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="G20" s="53"/>
-      <c r="H20" s="60" t="s">
-        <v>69</v>
-      </c>
-      <c r="I20" s="24"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="L20" s="24"/>
-      <c r="M20" s="25"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="25"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="L20" s="25"/>
+      <c r="M20" s="24"/>
       <c r="O20" s="1">
         <v>99</v>
       </c>
@@ -2150,29 +2150,29 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="46"/>
-      <c r="B21" s="48" t="s">
+      <c r="A21" s="35"/>
+      <c r="B21" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="24" t="s">
+      <c r="C21" s="37"/>
+      <c r="D21" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="48" t="s">
+      <c r="E21" s="25"/>
+      <c r="F21" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="53"/>
-      <c r="H21" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="I21" s="24"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="L21" s="24"/>
-      <c r="M21" s="25"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="25"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="L21" s="25"/>
+      <c r="M21" s="24"/>
       <c r="O21" s="1">
         <v>25</v>
       </c>
@@ -2181,27 +2181,27 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="49" t="s">
+      <c r="A22" s="36"/>
+      <c r="B22" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="49"/>
-      <c r="D22" s="52" t="s">
+      <c r="C22" s="38"/>
+      <c r="D22" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="52"/>
-      <c r="F22" s="52"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="62" t="s">
-        <v>71</v>
-      </c>
-      <c r="I22" s="52"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="L22" s="57"/>
-      <c r="M22" s="58"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="32"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="L22" s="26"/>
+      <c r="M22" s="27"/>
       <c r="O22" s="1">
         <v>4</v>
       </c>
@@ -2210,21 +2210,21 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="24"/>
       <c r="O23" s="1">
         <v>99</v>
       </c>
@@ -2233,90 +2233,99 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="28"/>
+      <c r="A24" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="58"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="59"/>
       <c r="P24" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+      <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="30"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="30"/>
-      <c r="J26" s="30"/>
-      <c r="K26" s="30"/>
-      <c r="L26" s="30"/>
-      <c r="M26" s="31"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="62"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21" t="s">
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="54"/>
+      <c r="E27" s="54"/>
+      <c r="F27" s="54"/>
+      <c r="G27" s="54"/>
+      <c r="H27" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="22"/>
+      <c r="I27" s="54"/>
+      <c r="J27" s="54"/>
+      <c r="K27" s="54"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:M2"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
@@ -2331,25 +2340,16 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:M2"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="A23:M23"/>
-    <mergeCell ref="A24:M24"/>
-    <mergeCell ref="A25:M25"/>
-    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
   </mergeCells>
   <conditionalFormatting sqref="E28:E1048576 E4:E17">
     <cfRule type="colorScale" priority="1">

</xml_diff>

<commit_message>
ADD - Other / Chimera Drop
</commit_message>
<xml_diff>
--- a/Event.xlsx
+++ b/Event.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aff98139d4bac41f/文件/DL/dragalia-data-track/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="266" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3D80C619-B7BC-4D6D-9BCB-1C5C81ED0368}"/>
+  <xr:revisionPtr revIDLastSave="283" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0761D126-0ED5-45BD-BFCA-F87653B99411}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="1080" windowWidth="20820" windowHeight="13890" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="13755" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
   </bookViews>
   <sheets>
     <sheet name="United Front" sheetId="1" r:id="rId1"/>
@@ -1310,8 +1310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D545DF4-55DC-4582-810A-BD07097A5744}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="A1:M27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
IMP - Miscellaneous Excel Improvements
</commit_message>
<xml_diff>
--- a/Event.xlsx
+++ b/Event.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aff98139d4bac41f/文件/DL/dragalia-data-track/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="283" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0761D126-0ED5-45BD-BFCA-F87653B99411}"/>
+  <xr:revisionPtr revIDLastSave="328" documentId="8_{2A9AB851-5500-4F1C-9CE2-EAEDD80398D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8E194961-A62D-4073-8F22-079F10FE4EBD}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="13755" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A4130D2B-1579-44EF-949A-AE9073E24CF9}"/>
   </bookViews>
   <sheets>
     <sheet name="United Front" sheetId="1" r:id="rId1"/>
+    <sheet name="Summer Saviors" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="77">
   <si>
     <t>初級</t>
   </si>
@@ -375,6 +376,24 @@
       </rPr>
       <t>06/13 5:23 AM CDT</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">迎擊戰 - 盛夏的假期守護者 簡表 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>06/13 5:23 AM CDT</t>
+    </r>
+  </si>
+  <si>
+    <t>150000 P</t>
   </si>
 </sst>
 </file>
@@ -745,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -804,24 +823,123 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -839,99 +957,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -999,6 +1024,61 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8658225" y="0"/>
+          <a:ext cx="457200" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAF159F3-7D24-41CC-9553-2EF2FBFA1CB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8362950" y="0"/>
           <a:ext cx="457200" cy="457200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1310,7 +1390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D545DF4-55DC-4582-810A-BD07097A5744}">
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
@@ -1326,61 +1406,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
-      <c r="M1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
     </row>
     <row r="2" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="52"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="45" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="47"/>
-      <c r="H3" s="45" t="s">
+      <c r="G3" s="41"/>
+      <c r="H3" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="47"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="41"/>
     </row>
     <row r="4" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
@@ -1428,7 +1508,7 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="42" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -1478,7 +1558,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -1526,7 +1606,7 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
@@ -1574,7 +1654,7 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="43" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1624,7 +1704,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="8" t="s">
         <v>6</v>
       </c>
@@ -1672,7 +1752,7 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
+      <c r="A10" s="43"/>
       <c r="B10" s="8" t="s">
         <v>7</v>
       </c>
@@ -1721,7 +1801,7 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="42" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1771,7 +1851,7 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
+      <c r="A12" s="42"/>
       <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
@@ -1819,7 +1899,7 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
+      <c r="A13" s="42"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1868,7 +1948,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
+      <c r="A14" s="43" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1884,10 +1964,10 @@
         <f t="shared" si="0"/>
         <v>187.5</v>
       </c>
-      <c r="F14" s="43" t="s">
+      <c r="F14" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="44">
+      <c r="G14" s="38">
         <f>SUM(O:O)/SUM(P:P)</f>
         <v>2.2682926829268291</v>
       </c>
@@ -1919,7 +1999,7 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="49"/>
+      <c r="A15" s="43"/>
       <c r="B15" s="8" t="s">
         <v>6</v>
       </c>
@@ -1933,8 +2013,8 @@
         <f t="shared" si="0"/>
         <v>222.22222222222223</v>
       </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="44"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="38"/>
       <c r="H15" s="9" t="s">
         <v>20</v>
       </c>
@@ -1963,7 +2043,7 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="49"/>
+      <c r="A16" s="43"/>
       <c r="B16" s="8" t="s">
         <v>7</v>
       </c>
@@ -1977,8 +2057,8 @@
         <f t="shared" si="0"/>
         <v>350</v>
       </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="44"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="38"/>
       <c r="H16" s="9" t="s">
         <v>21</v>
       </c>
@@ -2009,10 +2089,10 @@
       </c>
     </row>
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="41"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="6">
         <v>0</v>
       </c>
@@ -2059,27 +2139,27 @@
       </c>
     </row>
     <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="20" t="s">
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="I18" s="21"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="21" t="s">
+      <c r="I18" s="52"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="L18" s="21"/>
-      <c r="M18" s="28"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="61"/>
       <c r="O18" s="1">
         <v>20</v>
       </c>
@@ -2088,29 +2168,29 @@
       </c>
     </row>
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="35"/>
-      <c r="B19" s="25" t="s">
+      <c r="A19" s="48"/>
+      <c r="B19" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25" t="s">
+      <c r="C19" s="26"/>
+      <c r="D19" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="37" t="s">
+      <c r="E19" s="26"/>
+      <c r="F19" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="39"/>
-      <c r="H19" s="29" t="s">
+      <c r="G19" s="55"/>
+      <c r="H19" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="I19" s="25"/>
-      <c r="J19" s="30"/>
-      <c r="K19" s="23" t="s">
+      <c r="I19" s="26"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="L19" s="23"/>
-      <c r="M19" s="24"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="27"/>
       <c r="O19" s="1">
         <v>30</v>
       </c>
@@ -2119,29 +2199,29 @@
       </c>
     </row>
     <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="25" t="s">
+      <c r="A20" s="48"/>
+      <c r="B20" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25" t="s">
+      <c r="C20" s="26"/>
+      <c r="D20" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="37" t="s">
+      <c r="E20" s="26"/>
+      <c r="F20" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="G20" s="39"/>
-      <c r="H20" s="29" t="s">
+      <c r="G20" s="55"/>
+      <c r="H20" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="I20" s="25"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="25" t="s">
+      <c r="I20" s="26"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="L20" s="25"/>
-      <c r="M20" s="24"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="27"/>
       <c r="O20" s="1">
         <v>99</v>
       </c>
@@ -2150,29 +2230,29 @@
       </c>
     </row>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="35"/>
-      <c r="B21" s="37" t="s">
+      <c r="A21" s="48"/>
+      <c r="B21" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="25" t="s">
+      <c r="C21" s="50"/>
+      <c r="D21" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="37" t="s">
+      <c r="E21" s="26"/>
+      <c r="F21" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="39"/>
-      <c r="H21" s="29" t="s">
+      <c r="G21" s="55"/>
+      <c r="H21" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="I21" s="25"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="25" t="s">
+      <c r="I21" s="26"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="L21" s="25"/>
-      <c r="M21" s="24"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="27"/>
       <c r="O21" s="1">
         <v>25</v>
       </c>
@@ -2181,27 +2261,27 @@
       </c>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="36"/>
-      <c r="B22" s="38" t="s">
+      <c r="A22" s="49"/>
+      <c r="B22" s="51" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="38"/>
-      <c r="D22" s="32" t="s">
+      <c r="C22" s="51"/>
+      <c r="D22" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="31" t="s">
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="I22" s="32"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="26" t="s">
+      <c r="I22" s="54"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="L22" s="26"/>
-      <c r="M22" s="27"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="60"/>
       <c r="O22" s="1">
         <v>4</v>
       </c>
@@ -2210,21 +2290,21 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
+      <c r="A23" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="24"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="27"/>
       <c r="O23" s="1">
         <v>99</v>
       </c>
@@ -2233,99 +2313,90 @@
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="57" t="s">
+      <c r="A24" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="58"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="58"/>
-      <c r="L24" s="58"/>
-      <c r="M24" s="59"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="30"/>
       <c r="P24" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-      <c r="M25" s="24"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="27"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="60" t="s">
+      <c r="A26" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="62"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="33"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="54" t="s">
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="54"/>
-      <c r="M27" s="55"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="H27:M27"/>
-    <mergeCell ref="A23:M23"/>
-    <mergeCell ref="A24:M24"/>
-    <mergeCell ref="A25:M25"/>
-    <mergeCell ref="A26:M26"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="H22:J22"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B20:C20"/>
@@ -2340,16 +2411,1099 @@
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="F21:G21"/>
     <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A26:M26"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E28:E1048576 E4:E17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFFA9698"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFB1DFBD"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07FEAEC6-9FA8-4302-B2D6-4D56FD0C98A9}">
+  <dimension ref="A1:P27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" style="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="10.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+    </row>
+    <row r="2" spans="1:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="46"/>
+    </row>
+    <row r="3" spans="1:16" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="41"/>
+      <c r="H3" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="41"/>
+    </row>
+    <row r="4" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6">
+        <v>700</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" ref="E5:E16" si="0">D5/C5</f>
+        <v>233.33333333333334</v>
+      </c>
+      <c r="F5" s="9">
+        <v>700</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1</v>
+      </c>
+      <c r="J5" s="6">
+        <f>I5*D5</f>
+        <v>700</v>
+      </c>
+      <c r="K5" s="6">
+        <f>SUM($J$5:J5)</f>
+        <v>700</v>
+      </c>
+      <c r="L5" s="6">
+        <v>9</v>
+      </c>
+      <c r="M5" s="10">
+        <f>SUM($L$5:L5)</f>
+        <v>9</v>
+      </c>
+      <c r="O5" s="1">
+        <v>10</v>
+      </c>
+      <c r="P5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="42"/>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1500</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="0"/>
+        <v>375</v>
+      </c>
+      <c r="F6" s="9">
+        <v>2100</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6">
+        <f>I6*D6</f>
+        <v>1500</v>
+      </c>
+      <c r="K6" s="6">
+        <f>SUM($J$5:J6)</f>
+        <v>2200</v>
+      </c>
+      <c r="L6" s="6">
+        <v>12</v>
+      </c>
+      <c r="M6" s="10">
+        <f>SUM($L$5:L6)</f>
+        <v>21</v>
+      </c>
+      <c r="O6" s="1">
+        <v>27</v>
+      </c>
+      <c r="P6" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="42"/>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6">
+        <v>5</v>
+      </c>
+      <c r="D7" s="6">
+        <v>2000</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="F7" s="9">
+        <v>4200</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" ref="J7:J17" si="1">I7*D7</f>
+        <v>2000</v>
+      </c>
+      <c r="K7" s="6">
+        <f>SUM($J$5:J7)</f>
+        <v>4200</v>
+      </c>
+      <c r="L7" s="6">
+        <v>25</v>
+      </c>
+      <c r="M7" s="10">
+        <f>SUM($L$5:L7)</f>
+        <v>46</v>
+      </c>
+      <c r="O7" s="1">
+        <v>20</v>
+      </c>
+      <c r="P7" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="6">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1500</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="F8" s="9">
+        <v>6300</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="1"/>
+        <v>1500</v>
+      </c>
+      <c r="K8" s="6">
+        <f>SUM($J$5:J8)</f>
+        <v>5700</v>
+      </c>
+      <c r="L8" s="6">
+        <v>6</v>
+      </c>
+      <c r="M8" s="10">
+        <f>SUM($L$5:L8)</f>
+        <v>52</v>
+      </c>
+      <c r="O8" s="1">
+        <v>25</v>
+      </c>
+      <c r="P8" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="43"/>
+      <c r="B9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6">
+        <v>7</v>
+      </c>
+      <c r="D9" s="6">
+        <v>3000</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>428.57142857142856</v>
+      </c>
+      <c r="F9" s="9">
+        <v>17000</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+      <c r="K9" s="6">
+        <f>SUM($J$5:J9)</f>
+        <v>8700</v>
+      </c>
+      <c r="L9" s="6">
+        <v>7</v>
+      </c>
+      <c r="M9" s="10">
+        <f>SUM($L$5:L9)</f>
+        <v>59</v>
+      </c>
+      <c r="O9" s="1">
+        <v>23</v>
+      </c>
+      <c r="P9" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+      <c r="B10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
+        <v>625</v>
+      </c>
+      <c r="F10" s="9">
+        <v>25000</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="6">
+        <v>1</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="1"/>
+        <v>5000</v>
+      </c>
+      <c r="K10" s="6">
+        <f>SUM($J$5:J10)</f>
+        <v>13700</v>
+      </c>
+      <c r="L10" s="6">
+        <f>24*8</f>
+        <v>192</v>
+      </c>
+      <c r="M10" s="10">
+        <f>SUM($L$5:L10)</f>
+        <v>251</v>
+      </c>
+      <c r="O10" s="1">
+        <v>10</v>
+      </c>
+      <c r="P10" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6">
+        <v>4500</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+      <c r="F11" s="9">
+        <v>35000</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="6">
+        <v>1</v>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="1"/>
+        <v>4500</v>
+      </c>
+      <c r="K11" s="6">
+        <f>SUM($J$5:J11)</f>
+        <v>18200</v>
+      </c>
+      <c r="L11" s="6">
+        <v>10</v>
+      </c>
+      <c r="M11" s="10">
+        <f>SUM($L$5:L11)</f>
+        <v>261</v>
+      </c>
+      <c r="O11" s="1">
+        <v>30</v>
+      </c>
+      <c r="P11" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="42"/>
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="6">
+        <v>12</v>
+      </c>
+      <c r="D12" s="6">
+        <v>9000</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>750</v>
+      </c>
+      <c r="F12" s="11">
+        <v>700000</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="6">
+        <v>1</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="1"/>
+        <v>9000</v>
+      </c>
+      <c r="K12" s="6">
+        <f>SUM($J$5:J12)</f>
+        <v>27200</v>
+      </c>
+      <c r="L12" s="6">
+        <v>12</v>
+      </c>
+      <c r="M12" s="10">
+        <f>SUM($L$5:L12)</f>
+        <v>273</v>
+      </c>
+      <c r="O12" s="1">
+        <v>30</v>
+      </c>
+      <c r="P12" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="42"/>
+      <c r="B13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="6">
+        <v>14</v>
+      </c>
+      <c r="D13" s="6">
+        <v>12000</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>857.14285714285711</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="6">
+        <v>1</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="1"/>
+        <v>12000</v>
+      </c>
+      <c r="K13" s="6">
+        <f>SUM($J$5:J13)</f>
+        <v>39200</v>
+      </c>
+      <c r="L13" s="6">
+        <f>14*19</f>
+        <v>266</v>
+      </c>
+      <c r="M13" s="10">
+        <f>SUM($L$5:L13)</f>
+        <v>539</v>
+      </c>
+      <c r="O13" s="1">
+        <v>30</v>
+      </c>
+      <c r="P13" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="6">
+        <v>16</v>
+      </c>
+      <c r="D14" s="6">
+        <v>10000</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
+        <v>625</v>
+      </c>
+      <c r="F14" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="38">
+        <f>SUM(O:O)/SUM(P:P)</f>
+        <v>2.2682926829268291</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="6">
+        <v>1</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="1"/>
+        <v>10000</v>
+      </c>
+      <c r="K14" s="6">
+        <f>SUM($J$5:J14)</f>
+        <v>49200</v>
+      </c>
+      <c r="L14" s="6">
+        <v>16</v>
+      </c>
+      <c r="M14" s="10">
+        <f>SUM($L$5:L14)</f>
+        <v>555</v>
+      </c>
+      <c r="O14" s="1">
+        <v>30</v>
+      </c>
+      <c r="P14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="43"/>
+      <c r="B15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6">
+        <v>18</v>
+      </c>
+      <c r="D15" s="6">
+        <v>30000</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="0"/>
+        <v>1666.6666666666667</v>
+      </c>
+      <c r="F15" s="34"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="6">
+        <v>1</v>
+      </c>
+      <c r="J15" s="6">
+        <f t="shared" si="1"/>
+        <v>30000</v>
+      </c>
+      <c r="K15" s="6">
+        <f>SUM($J$5:J15)</f>
+        <v>79200</v>
+      </c>
+      <c r="L15" s="6">
+        <v>18</v>
+      </c>
+      <c r="M15" s="10">
+        <f>SUM($L$5:L15)</f>
+        <v>573</v>
+      </c>
+      <c r="O15" s="1">
+        <v>99</v>
+      </c>
+      <c r="P15" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="43"/>
+      <c r="B16" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="6">
+        <v>20</v>
+      </c>
+      <c r="D16" s="6">
+        <v>50000</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="F16" s="34"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="6">
+        <v>1</v>
+      </c>
+      <c r="J16" s="6">
+        <f t="shared" si="1"/>
+        <v>50000</v>
+      </c>
+      <c r="K16" s="6">
+        <f>SUM($J$5:J16)</f>
+        <v>129200</v>
+      </c>
+      <c r="L16" s="6">
+        <f>I16*C16</f>
+        <v>20</v>
+      </c>
+      <c r="M16" s="10">
+        <f>SUM($L$5:L16)</f>
+        <v>593</v>
+      </c>
+      <c r="O16" s="1">
+        <v>30</v>
+      </c>
+      <c r="P16" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="35"/>
+      <c r="C17" s="6">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6">
+        <v>147000</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="10">
+        <f>SUM(O:O)</f>
+        <v>651</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="6">
+        <f>_xlfn.FLOOR.MATH(I16/G14)</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="6">
+        <f>SUM($J$5:J17)</f>
+        <v>129200</v>
+      </c>
+      <c r="L17" s="6">
+        <v>0</v>
+      </c>
+      <c r="M17" s="10">
+        <f>SUM($L$5:L17)</f>
+        <v>593</v>
+      </c>
+      <c r="O17" s="1">
+        <v>10</v>
+      </c>
+      <c r="P17" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="52" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="52"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="52" t="s">
+        <v>65</v>
+      </c>
+      <c r="L18" s="52"/>
+      <c r="M18" s="61"/>
+      <c r="O18" s="1">
+        <v>20</v>
+      </c>
+      <c r="P18" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="48"/>
+      <c r="B19" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="26"/>
+      <c r="F19" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="55"/>
+      <c r="H19" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="I19" s="26"/>
+      <c r="J19" s="63"/>
+      <c r="K19" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="L19" s="58"/>
+      <c r="M19" s="27"/>
+      <c r="O19" s="1">
+        <v>30</v>
+      </c>
+      <c r="P19" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="48"/>
+      <c r="B20" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="26"/>
+      <c r="F20" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="55"/>
+      <c r="H20" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="26"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="L20" s="26"/>
+      <c r="M20" s="27"/>
+      <c r="O20" s="1">
+        <v>99</v>
+      </c>
+      <c r="P20" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="48"/>
+      <c r="B21" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="50"/>
+      <c r="D21" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="26"/>
+      <c r="F21" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="55"/>
+      <c r="H21" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="26"/>
+      <c r="J21" s="63"/>
+      <c r="K21" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="L21" s="26"/>
+      <c r="M21" s="27"/>
+      <c r="O21" s="1">
+        <v>25</v>
+      </c>
+      <c r="P21" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="49"/>
+      <c r="B22" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="51"/>
+      <c r="D22" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="56"/>
+      <c r="H22" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="I22" s="54"/>
+      <c r="J22" s="56"/>
+      <c r="K22" s="59" t="s">
+        <v>63</v>
+      </c>
+      <c r="L22" s="59"/>
+      <c r="M22" s="60"/>
+      <c r="O22" s="1">
+        <v>4</v>
+      </c>
+      <c r="P22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="27"/>
+      <c r="O23" s="1">
+        <v>99</v>
+      </c>
+      <c r="P23" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="30"/>
+      <c r="P24" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="26"/>
+      <c r="K25" s="26"/>
+      <c r="L25" s="26"/>
+      <c r="M25" s="27"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="33"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="43">
+    <mergeCell ref="A24:M24"/>
+    <mergeCell ref="A25:M25"/>
+    <mergeCell ref="A26:M26"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="H27:M27"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="A23:M23"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:G18"/>
     <mergeCell ref="H18:J18"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="K19:M19"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:M3"/>
   </mergeCells>
   <conditionalFormatting sqref="E28:E1048576 E4:E17">
     <cfRule type="colorScale" priority="1">

</xml_diff>